<commit_message>
fixes and improvements to profiles for HCIM Infusion
</commit_message>
<xml_diff>
--- a/Profiles-Staging/Infusion - STU3.xlsx
+++ b/Profiles-Staging/Infusion - STU3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="135">
   <si>
     <t>Concept</t>
   </si>
@@ -406,9 +406,6 @@
 Central lines can contain one or more lumens; peripheral infusions do not have lumens and only have one line.</t>
   </si>
   <si>
-    <t>Dit wordt het hoofdconcept, afgeleid van MedicalDevice. Er staat wel 0..1, komt het voor dat er een infuus is, waarbij geen Catheter is? (zo ja, dan kan het niet op deze manier)</t>
-  </si>
-  <si>
     <t>DeviceUseStatement.extension:LumenOrLine(complex)</t>
   </si>
   <si>
@@ -431,6 +428,12 @@
   </si>
   <si>
     <t>MedicationAdministration.device.extension:MedicalDevice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dit wordt het hoofdconcept, afgeleid van MedicalDevice. Er staat wel 0..1, komt het voor dat er een infuus is, waarbij geen Catheter is? (zo ja, dan kan het niet op deze manier) </t>
+  </si>
+  <si>
+    <t>AT: of een verwijzing naar een 'standaard' infuus device</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -701,11 +704,17 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1058,30 +1067,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q14"/>
+  <dimension ref="B2:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="6" width="2" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.09765625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="16.09765625" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="75" customWidth="1"/>
-    <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" customWidth="1"/>
-    <col min="17" max="17" width="47.42578125" customWidth="1"/>
-    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="93.19921875" customWidth="1"/>
+    <col min="14" max="14" width="52.8984375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="84.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="61.19921875" style="30" customWidth="1"/>
+    <col min="18" max="18" width="48.8984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,11 +1132,11 @@
       <c r="P2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" ht="26" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>42</v>
       </c>
@@ -1153,7 +1168,7 @@
       </c>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="2:17" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" ht="43.5" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>47</v>
@@ -1188,10 +1203,13 @@
         <v>15</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="R4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
@@ -1225,7 +1243,7 @@
       </c>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>25</v>
@@ -1261,7 +1279,7 @@
       </c>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" ht="52" x14ac:dyDescent="0.3">
       <c r="B7" s="21"/>
       <c r="C7" s="22" t="s">
         <v>54</v>
@@ -1289,11 +1307,11 @@
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
       <c r="P7" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="25"/>
     </row>
-    <row r="8" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" ht="26" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
@@ -1325,11 +1343,11 @@
         <v>63</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" ht="26" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
@@ -1361,11 +1379,11 @@
         <v>69</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
@@ -1395,11 +1413,11 @@
         <v>24</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="2:17" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" ht="52" x14ac:dyDescent="0.3">
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22" t="s">
@@ -1427,11 +1445,11 @@
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
       <c r="P11" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q11" s="25"/>
     </row>
-    <row r="12" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" ht="26" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1463,11 +1481,11 @@
         <v>24</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" ht="26" x14ac:dyDescent="0.3">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1499,11 +1517,11 @@
         <v>14</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1535,7 +1553,7 @@
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q14" s="10"/>
     </row>
@@ -1562,29 +1580,29 @@
       <selection activeCell="E22" sqref="E22:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="1" max="2" width="8.59765625" customWidth="1"/>
+    <col min="3" max="3" width="41.296875" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.8984375" customWidth="1"/>
+    <col min="7" max="7" width="27.09765625" customWidth="1"/>
+    <col min="8" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="27" t="s">
+    <row r="3" spans="3:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="27" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="18" t="s">
         <v>30</v>
       </c>
@@ -1601,7 +1619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
         <v>94</v>
       </c>
@@ -1618,7 +1636,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
         <v>96</v>
       </c>
@@ -1635,7 +1653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
         <v>98</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
         <v>100</v>
       </c>
@@ -1669,7 +1687,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="14" t="s">
         <v>102</v>
       </c>
@@ -1686,7 +1704,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="14" t="s">
         <v>104</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="14" t="s">
         <v>106</v>
       </c>
@@ -1720,7 +1738,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
@@ -1737,18 +1755,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="27" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" s="18" t="s">
         <v>30</v>
       </c>
@@ -1765,7 +1783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" ht="26" x14ac:dyDescent="0.3">
       <c r="C17" s="14" t="s">
         <v>110</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:7" ht="26" x14ac:dyDescent="0.3">
       <c r="C18" s="14" t="s">
         <v>114</v>
       </c>
@@ -1799,7 +1817,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="14" t="s">
         <v>37</v>
       </c>
@@ -1816,18 +1834,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="27" t="s">
+      <c r="D22" s="29"/>
+      <c r="E22" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="18" t="s">
         <v>30</v>
       </c>
@@ -1844,7 +1862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="14" t="s">
         <v>118</v>
       </c>
@@ -1861,7 +1879,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="14" t="s">
         <v>120</v>
       </c>
@@ -1878,7 +1896,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="14" t="s">
         <v>122</v>
       </c>

</xml_diff>